<commit_message>
create and write functionality (from home)
</commit_message>
<xml_diff>
--- a/output/test.xlsx
+++ b/output/test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>Покупатель</t>
   </si>
@@ -47,24 +48,133 @@
   </si>
   <si>
     <t>Статус товара</t>
+  </si>
+  <si>
+    <t>asfasf</t>
+  </si>
+  <si>
+    <t>566</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>safas</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>005566</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Иван Ургант</t>
+  </si>
+  <si>
+    <t>226655</t>
+  </si>
+  <si>
+    <t>07-05-2018</t>
+  </si>
+  <si>
+    <t>226600</t>
+  </si>
+  <si>
+    <t>Шутки</t>
+  </si>
+  <si>
+    <t>003654</t>
+  </si>
+  <si>
+    <t>Потеряны</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Наполеон Бонапарт</t>
+  </si>
+  <si>
+    <t>-666</t>
+  </si>
+  <si>
+    <t>01-02-1812</t>
+  </si>
+  <si>
+    <t>0077ff</t>
+  </si>
+  <si>
+    <t>Французкая армия</t>
+  </si>
+  <si>
+    <t>0066988</t>
+  </si>
+  <si>
+    <t>Замерзла</t>
+  </si>
+  <si>
+    <t>Adolf Hitler</t>
+  </si>
+  <si>
+    <t>09-05-1945</t>
+  </si>
+  <si>
+    <t>1945</t>
+  </si>
+  <si>
+    <t>Немецкая армия</t>
+  </si>
+  <si>
+    <t>006666</t>
+  </si>
+  <si>
+    <t>RIP</t>
+  </si>
+  <si>
+    <t>Микки Маус</t>
+  </si>
+  <si>
+    <t>555777</t>
+  </si>
+  <si>
+    <t>06-05-2018</t>
+  </si>
+  <si>
+    <t>5665</t>
+  </si>
+  <si>
+    <t>Волшебные краски</t>
+  </si>
+  <si>
+    <t>003365</t>
+  </si>
+  <si>
+    <t>Высохли</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -80,16 +190,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -377,12 +486,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -419,7 +535,152 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Many items in 'goods' logic solving (from work)
</commit_message>
<xml_diff>
--- a/output/test.xlsx
+++ b/output/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
   <si>
     <t>Покупатель</t>
   </si>
@@ -156,6 +156,27 @@
   </si>
   <si>
     <t>Высохли</t>
+  </si>
+  <si>
+    <t>Вильям Иванович Шекспир</t>
+  </si>
+  <si>
+    <t>20-05-1456</t>
+  </si>
+  <si>
+    <t>29654</t>
+  </si>
+  <si>
+    <t>Гамлет</t>
+  </si>
+  <si>
+    <t>1шт</t>
+  </si>
+  <si>
+    <t>006312</t>
+  </si>
+  <si>
+    <t>Долго не живет</t>
   </si>
 </sst>
 </file>
@@ -491,7 +512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -680,6 +701,35 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Decompasition some functions (from home)
</commit_message>
<xml_diff>
--- a/output/test.xlsx
+++ b/output/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>Покупатель</t>
   </si>
@@ -177,6 +177,39 @@
   </si>
   <si>
     <t>Долго не живет</t>
+  </si>
+  <si>
+    <t>Клемент Ворошилов</t>
+  </si>
+  <si>
+    <t>02051945</t>
+  </si>
+  <si>
+    <t>Винтовка Мосина</t>
+  </si>
+  <si>
+    <t>1шт на взвод</t>
+  </si>
+  <si>
+    <t>Не стреляет, но колит</t>
+  </si>
+  <si>
+    <t>Жуков Георгий</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>Пленные Немцы</t>
+  </si>
+  <si>
+    <t>40 полков</t>
+  </si>
+  <si>
+    <t>001945</t>
+  </si>
+  <si>
+    <t>Плохо работают</t>
   </si>
 </sst>
 </file>
@@ -512,7 +545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -730,6 +763,64 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
.gitignore editting (from work)
</commit_message>
<xml_diff>
--- a/output/test.xlsx
+++ b/output/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Покупатель</t>
   </si>
@@ -48,27 +48,6 @@
   </si>
   <si>
     <t>Статус товара</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>qwe</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>еку</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
 </sst>
 </file>
@@ -404,14 +383,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="35"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="16"/>
+    <col customWidth="1" max="4" min="4" width="11"/>
+    <col customWidth="1" max="5" min="5" width="35"/>
+    <col customWidth="1" max="6" min="6" width="12"/>
+    <col customWidth="1" max="7" min="7" width="18"/>
+    <col customWidth="1" max="8" min="8" width="35"/>
+    <col customWidth="1" max="9" min="9" width="22"/>
+    <col customWidth="1" max="10" min="10" width="22"/>
+    <col customWidth="1" max="11" min="11" width="22"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -447,111 +439,6 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>